<commit_message>
Add population data for 2011
</commit_message>
<xml_diff>
--- a/Data/MASTER_DATA.xlsx
+++ b/Data/MASTER_DATA.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="40" windowWidth="23000" windowHeight="10040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterate="1" iterateCount="1000" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>County</t>
   </si>
@@ -216,9 +221,6 @@
     <t>Median family income</t>
   </si>
   <si>
-    <t>Population</t>
-  </si>
-  <si>
     <t>Humber of households</t>
   </si>
   <si>
@@ -235,6 +237,9 @@
   </si>
   <si>
     <t>long</t>
+  </si>
+  <si>
+    <t>Population 2011</t>
   </si>
 </sst>
 </file>
@@ -272,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -280,17 +285,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
@@ -593,26 +630,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,29 +663,32 @@
       <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -660,29 +701,32 @@
       <c r="D2">
         <v>76159</v>
       </c>
-      <c r="E2">
-        <v>304204</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="5">
+        <v>303889</v>
+      </c>
+      <c r="F2" s="5">
+        <v>303565</v>
+      </c>
+      <c r="G2">
         <v>126251</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>3740.3</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>402</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>3338.3</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>42.619625812500047</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>-73.928693449999884</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -695,29 +739,32 @@
       <c r="D3">
         <v>49864</v>
       </c>
-      <c r="E3">
-        <v>48946</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="5">
+        <v>48951</v>
+      </c>
+      <c r="F3" s="5">
+        <v>48778</v>
+      </c>
+      <c r="G3">
         <v>18208</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>1720.5</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>183.4</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>1537.2</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>42.242916785714286</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>-78.06125200000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -730,29 +777,32 @@
       <c r="D4">
         <v>38431</v>
       </c>
-      <c r="E4">
-        <v>1385108</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="5">
+        <v>1387159</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1392002</v>
+      </c>
+      <c r="G4">
         <v>483449</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>2450.1999999999998</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>869.6</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>1580.6</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>40.847427500000009</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>-73.875928192307683</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -765,29 +815,32 @@
       <c r="D5">
         <v>57545</v>
       </c>
-      <c r="E5">
-        <v>200600</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="5">
+        <v>200368</v>
+      </c>
+      <c r="F5" s="5">
+        <v>199031</v>
+      </c>
+      <c r="G5">
         <v>82167</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>3233.6</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>260</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>2973.5</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>42.180092000000009</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>-75.846758451612914</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -800,29 +853,32 @@
       <c r="D6">
         <v>51227</v>
       </c>
-      <c r="E6">
-        <v>80317</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="5">
+        <v>80250</v>
+      </c>
+      <c r="F6" s="5">
+        <v>79832</v>
+      </c>
+      <c r="G6">
         <v>32263</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>2614.8000000000002</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>236.3</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>2378.5</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>42.298554363636363</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>-78.680371363636368</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -835,29 +891,32 @@
       <c r="D7">
         <v>58761</v>
       </c>
-      <c r="E7">
-        <v>80026</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="5">
+        <v>79997</v>
+      </c>
+      <c r="F7" s="5">
+        <v>79738</v>
+      </c>
+      <c r="G7">
         <v>31445</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>2250</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>201.5</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>2048.5</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>42.948406157894745</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>-76.581230105263145</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -870,29 +929,32 @@
       <c r="D8">
         <v>51031</v>
       </c>
-      <c r="E8">
-        <v>134905</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="5">
+        <v>134813</v>
+      </c>
+      <c r="F8" s="5">
+        <v>134368</v>
+      </c>
+      <c r="G8">
         <v>54244</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>2939.6</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>237.4</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>2702.2</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>42.257775949999981</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>-79.357110599999984</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -905,29 +967,32 @@
       <c r="D9">
         <v>55246</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>88830</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
+        <v>88840</v>
+      </c>
+      <c r="G9">
         <v>35462</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>2388.8000000000002</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>233.1</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>2155.6999999999998</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>42.138061888888885</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>-76.781497500000015</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -940,29 +1005,32 @@
       <c r="D10">
         <v>52229</v>
       </c>
-      <c r="E10">
-        <v>50477</v>
-      </c>
-      <c r="F10">
+      <c r="E10" s="5">
+        <v>50396</v>
+      </c>
+      <c r="F10" s="5">
+        <v>50118</v>
+      </c>
+      <c r="G10">
         <v>20436</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>1952.9</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>108</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>1844.8</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>42.529631999999999</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>-75.604708545454528</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -975,29 +1043,32 @@
       <c r="D11">
         <v>60280</v>
       </c>
-      <c r="E11">
-        <v>82128</v>
-      </c>
-      <c r="F11">
+      <c r="E11" s="5">
+        <v>82143</v>
+      </c>
+      <c r="F11" s="5">
+        <v>81945</v>
+      </c>
+      <c r="G11">
         <v>31582</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>2261.5</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>107.6</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>2154</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>44.750831439999999</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>-73.682668039999996</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1010,29 +1081,32 @@
       <c r="D12">
         <v>69132</v>
       </c>
-      <c r="E12">
-        <v>63096</v>
-      </c>
-      <c r="F12">
+      <c r="E12" s="5">
+        <v>63020</v>
+      </c>
+      <c r="F12" s="5">
+        <v>62550</v>
+      </c>
+      <c r="G12">
         <v>25906</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>1865.6</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>144.80000000000001</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>1720.8</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <v>42.287083969696965</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <v>-73.627775363636346</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1045,29 +1119,32 @@
       <c r="D13">
         <v>57743</v>
       </c>
-      <c r="E13">
-        <v>49336</v>
-      </c>
-      <c r="F13">
+      <c r="E13" s="5">
+        <v>49324</v>
+      </c>
+      <c r="F13" s="5">
+        <v>49363</v>
+      </c>
+      <c r="G13">
         <v>18671</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>2248.9</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>137.1</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>2111.8000000000002</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>42.601857750000001</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <v>-76.081791999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1080,29 +1157,32 @@
       <c r="D14">
         <v>53590</v>
       </c>
-      <c r="E14">
-        <v>47980</v>
-      </c>
-      <c r="F14">
+      <c r="E14" s="5">
+        <v>47843</v>
+      </c>
+      <c r="F14" s="5">
+        <v>47559</v>
+      </c>
+      <c r="G14">
         <v>19898</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>1734.2</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>138.6</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>1595.6</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>42.235073714285711</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <v>-74.882393085714284</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1115,29 +1195,32 @@
       <c r="D15">
         <v>83599</v>
       </c>
-      <c r="E15">
-        <v>297488</v>
-      </c>
-      <c r="F15">
+      <c r="E15" s="5">
+        <v>297739</v>
+      </c>
+      <c r="F15" s="5">
+        <v>297999</v>
+      </c>
+      <c r="G15">
         <v>107965</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>1949.6</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>243.9</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>1705.8</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>41.765817102564121</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>-73.757327820512828</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1150,29 +1233,32 @@
       <c r="D16">
         <v>63404</v>
       </c>
-      <c r="E16">
-        <v>919040</v>
-      </c>
-      <c r="F16">
+      <c r="E16" s="5">
+        <v>918751</v>
+      </c>
+      <c r="F16" s="5">
+        <v>918028</v>
+      </c>
+      <c r="G16">
         <v>383164</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>3637.5</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>505.8</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>3131.6</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>42.808838413793069</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>-78.790871885057427</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1185,29 +1271,32 @@
       <c r="D17">
         <v>55781</v>
       </c>
-      <c r="E17">
-        <v>39370</v>
-      </c>
-      <c r="F17">
+      <c r="E17" s="5">
+        <v>39316</v>
+      </c>
+      <c r="F17" s="5">
+        <v>39181</v>
+      </c>
+      <c r="G17">
         <v>16262</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>1454.2</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>102.9</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>1351.4</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>44.133381000000014</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>-73.667499806451616</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1220,29 +1309,32 @@
       <c r="D18">
         <v>50816</v>
       </c>
-      <c r="E18">
-        <v>51599</v>
-      </c>
-      <c r="F18">
+      <c r="E18" s="5">
+        <v>51609</v>
+      </c>
+      <c r="F18" s="5">
+        <v>51551</v>
+      </c>
+      <c r="G18">
         <v>19054</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>1897.9</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>114.8</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>1783.1</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <v>44.724345772727283</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <v>-74.354640954545459</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1255,29 +1347,32 @@
       <c r="D19">
         <v>50425</v>
       </c>
-      <c r="E19">
-        <v>55531</v>
-      </c>
-      <c r="F19">
+      <c r="E19" s="5">
+        <v>55471</v>
+      </c>
+      <c r="F19" s="5">
+        <v>55180</v>
+      </c>
+      <c r="G19">
         <v>22554</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>3108</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>226.3</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>2881.6</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <v>43.134699000000005</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>-74.357548428571434</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1290,29 +1385,32 @@
       <c r="D20">
         <v>60127</v>
       </c>
-      <c r="E20">
-        <v>60079</v>
-      </c>
-      <c r="F20">
+      <c r="E20" s="5">
+        <v>60080</v>
+      </c>
+      <c r="F20" s="5">
+        <v>59993</v>
+      </c>
+      <c r="G20">
         <v>23728</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>2572.5</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>188.1</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>2384.3000000000002</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
         <v>42.99312066666667</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <v>-78.17001622222223</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1325,29 +1423,32 @@
       <c r="D21">
         <v>55260</v>
       </c>
-      <c r="E21">
-        <v>49221</v>
-      </c>
-      <c r="F21">
+      <c r="E21" s="5">
+        <v>49160</v>
+      </c>
+      <c r="F21" s="5">
+        <v>48954</v>
+      </c>
+      <c r="G21">
         <v>19823</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>1691.5</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>189.8</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>1501.7</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
         <v>42.303304444444443</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L21" s="1">
         <v>-74.085482027777786</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1360,29 +1461,32 @@
       <c r="D22">
         <v>59911</v>
       </c>
-      <c r="E22">
-        <v>4836</v>
-      </c>
-      <c r="F22">
+      <c r="E22" s="5">
+        <v>4835</v>
+      </c>
+      <c r="F22" s="5">
+        <v>4793</v>
+      </c>
+      <c r="G22">
         <v>2262</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>1077.9000000000001</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>82.9</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <v>995</v>
       </c>
-      <c r="J22" s="1">
+      <c r="K22" s="1">
         <v>43.679319181818187</v>
       </c>
-      <c r="K22" s="1">
+      <c r="L22" s="1">
         <v>-74.449946454545454</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1395,29 +1499,32 @@
       <c r="D23">
         <v>53288</v>
       </c>
-      <c r="E23">
-        <v>64519</v>
-      </c>
-      <c r="F23">
+      <c r="E23" s="5">
+        <v>64481</v>
+      </c>
+      <c r="F23" s="5">
+        <v>64160</v>
+      </c>
+      <c r="G23">
         <v>26324</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>2209.4</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>269</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <v>1940.3</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <v>43.204288176470591</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L23" s="1">
         <v>-74.963219705882352</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1430,29 +1537,32 @@
       <c r="D24">
         <v>51834</v>
       </c>
-      <c r="E24">
-        <v>116229</v>
-      </c>
-      <c r="F24">
+      <c r="E24" s="5">
+        <v>116680</v>
+      </c>
+      <c r="F24" s="5">
+        <v>117910</v>
+      </c>
+      <c r="G24">
         <v>43451</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>2052.8000000000002</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>183.7</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>1869.1</v>
       </c>
-      <c r="J24" s="1">
+      <c r="K24" s="1">
         <v>44.027018142857138</v>
       </c>
-      <c r="K24" s="1">
+      <c r="L24" s="1">
         <v>-75.940387547619068</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1465,29 +1575,32 @@
       <c r="D25">
         <v>48777</v>
       </c>
-      <c r="E25">
-        <v>2504700</v>
-      </c>
-      <c r="F25">
+      <c r="E25" s="5">
+        <v>2508515</v>
+      </c>
+      <c r="F25" s="5">
+        <v>2532645</v>
+      </c>
+      <c r="G25">
         <v>916856</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>2242</v>
       </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
         <v>647.6</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <v>1594.4</v>
       </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <v>40.65298386538462</v>
       </c>
-      <c r="K25" s="1">
+      <c r="L25" s="1">
         <v>-73.952164750000037</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1500,29 +1613,32 @@
       <c r="D26">
         <v>49554</v>
       </c>
-      <c r="E26">
-        <v>27087</v>
-      </c>
-      <c r="F26">
+      <c r="E26" s="5">
+        <v>27101</v>
+      </c>
+      <c r="F26" s="5">
+        <v>27072</v>
+      </c>
+      <c r="G26">
         <v>10514</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>1787.9</v>
       </c>
-      <c r="H26" s="2">
+      <c r="I26" s="2">
         <v>97</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <v>1690.9</v>
       </c>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
         <v>43.764007588235302</v>
       </c>
-      <c r="K26" s="1">
+      <c r="L26" s="1">
         <v>-75.466915470588248</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1535,29 +1651,32 @@
       <c r="D27">
         <v>63539</v>
       </c>
-      <c r="E27">
-        <v>65393</v>
-      </c>
-      <c r="F27">
+      <c r="E27" s="5">
+        <v>65349</v>
+      </c>
+      <c r="F27" s="5">
+        <v>65070</v>
+      </c>
+      <c r="G27">
         <v>24409</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>1862.3</v>
       </c>
-      <c r="H27" s="2">
+      <c r="I27" s="2">
         <v>75.8</v>
       </c>
-      <c r="I27" s="2">
+      <c r="J27" s="2">
         <v>1786.5</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <v>42.750729999999997</v>
       </c>
-      <c r="K27" s="1">
+      <c r="L27" s="1">
         <v>-77.77631734782608</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1570,29 +1689,32 @@
       <c r="D28">
         <v>61828</v>
       </c>
-      <c r="E28">
-        <v>73442</v>
-      </c>
-      <c r="F28">
+      <c r="E28" s="5">
+        <v>73464</v>
+      </c>
+      <c r="F28" s="5">
+        <v>73365</v>
+      </c>
+      <c r="G28">
         <v>27754</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>1763.9</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>70.8</v>
       </c>
-      <c r="I28" s="2">
+      <c r="J28" s="2">
         <v>1693.1</v>
       </c>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
         <v>42.920524173913037</v>
       </c>
-      <c r="K28" s="1">
+      <c r="L28" s="1">
         <v>-75.674258999999978</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1605,29 +1727,32 @@
       <c r="D29">
         <v>65240</v>
       </c>
-      <c r="E29">
-        <v>744344</v>
-      </c>
-      <c r="F29">
+      <c r="E29" s="5">
+        <v>744635</v>
+      </c>
+      <c r="F29" s="5">
+        <v>745625</v>
+      </c>
+      <c r="G29">
         <v>300422</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>3586.2</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>389.1</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>3197.1</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <v>43.189400417910441</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="1">
         <v>-77.658262014925469</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1640,29 +1765,32 @@
       <c r="D30">
         <v>53476</v>
       </c>
-      <c r="E30">
-        <v>50219</v>
-      </c>
-      <c r="F30">
+      <c r="E30" s="5">
+        <v>50260</v>
+      </c>
+      <c r="F30" s="5">
+        <v>49916</v>
+      </c>
+      <c r="G30">
         <v>20272</v>
       </c>
-      <c r="G30" s="2">
+      <c r="H30" s="2">
         <v>2424.5</v>
       </c>
-      <c r="H30" s="2">
+      <c r="I30" s="2">
         <v>150.1</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>2274.4</v>
       </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
         <v>42.916339666666666</v>
       </c>
-      <c r="K30" s="1">
+      <c r="L30" s="1">
         <v>-74.418142266666692</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1675,29 +1803,32 @@
       <c r="D31">
         <v>107934</v>
       </c>
-      <c r="E31">
-        <v>1339532</v>
-      </c>
-      <c r="F31">
+      <c r="E31" s="5">
+        <v>1341033</v>
+      </c>
+      <c r="F31" s="5">
+        <v>1344436</v>
+      </c>
+      <c r="G31">
         <v>448528</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>1510.8</v>
       </c>
-      <c r="H31" s="2">
+      <c r="I31" s="2">
         <v>174.2</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>1336.6</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <v>40.72354783636365</v>
       </c>
-      <c r="K31" s="1">
+      <c r="L31" s="1">
         <v>-73.614297327272723</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1710,29 +1841,32 @@
       <c r="D32">
         <v>75629</v>
       </c>
-      <c r="E32">
-        <v>1585873</v>
-      </c>
-      <c r="F32">
+      <c r="E32" s="5">
+        <v>1587481</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1601948</v>
+      </c>
+      <c r="G32">
         <v>763846</v>
       </c>
-      <c r="G32" s="2">
+      <c r="H32" s="2">
         <v>3170</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>545.6</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>2624.4</v>
       </c>
-      <c r="J32" s="1">
+      <c r="K32" s="1">
         <v>40.767756487654331</v>
       </c>
-      <c r="K32" s="1">
+      <c r="L32" s="1">
         <v>-73.978840672839496</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1745,29 +1879,32 @@
       <c r="D33">
         <v>59471</v>
       </c>
-      <c r="E33">
-        <v>216469</v>
-      </c>
-      <c r="F33">
+      <c r="E33" s="5">
+        <v>216542</v>
+      </c>
+      <c r="F33" s="5">
+        <v>216011</v>
+      </c>
+      <c r="G33">
         <v>90556</v>
       </c>
-      <c r="G33" s="3">
+      <c r="H33" s="3">
         <v>3375.4</v>
       </c>
-      <c r="H33" s="3">
+      <c r="I33" s="3">
         <v>392.2</v>
       </c>
-      <c r="I33" s="3">
+      <c r="J33" s="3">
         <v>2983.2</v>
       </c>
-      <c r="J33" s="4">
+      <c r="K33" s="4">
         <v>43.228771478260867</v>
       </c>
-      <c r="K33" s="4">
+      <c r="L33" s="4">
         <v>-78.822577565217387</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1780,29 +1917,32 @@
       <c r="D34">
         <v>58017</v>
       </c>
-      <c r="E34">
-        <v>234878</v>
-      </c>
-      <c r="F34">
+      <c r="E34" s="5">
+        <v>234870</v>
+      </c>
+      <c r="F34" s="5">
+        <v>234287</v>
+      </c>
+      <c r="G34">
         <v>93028</v>
       </c>
-      <c r="G34" s="2">
+      <c r="H34" s="2">
         <v>2726</v>
       </c>
-      <c r="H34" s="2">
+      <c r="I34" s="2">
         <v>256.10000000000002</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>2470</v>
       </c>
-      <c r="J34" s="1">
+      <c r="K34" s="1">
         <v>43.161784052631575</v>
       </c>
-      <c r="K34" s="1">
+      <c r="L34" s="1">
         <v>-75.394030192982456</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1815,29 +1955,32 @@
       <c r="D35">
         <v>65929</v>
       </c>
-      <c r="E35">
-        <v>467026</v>
-      </c>
-      <c r="F35">
+      <c r="E35" s="5">
+        <v>467253</v>
+      </c>
+      <c r="F35" s="5">
+        <v>466960</v>
+      </c>
+      <c r="G35">
         <v>187686</v>
       </c>
-      <c r="G35" s="2">
+      <c r="H35" s="2">
         <v>2893.1</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>357.9</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="2">
         <v>2535.3000000000002</v>
       </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
         <v>43.029397299999964</v>
       </c>
-      <c r="K35" s="1">
+      <c r="L35" s="1">
         <v>-76.177859516666658</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1850,29 +1993,32 @@
       <c r="D36">
         <v>69877</v>
       </c>
-      <c r="E36">
-        <v>107931</v>
-      </c>
-      <c r="F36">
+      <c r="E36" s="5">
+        <v>108095</v>
+      </c>
+      <c r="F36" s="5">
+        <v>108525</v>
+      </c>
+      <c r="G36">
         <v>43019</v>
       </c>
-      <c r="G36" s="2">
+      <c r="H36" s="2">
         <v>1897.9</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>121.9</v>
       </c>
-      <c r="I36" s="2">
+      <c r="J36" s="2">
         <v>1776</v>
       </c>
-      <c r="J36" s="1">
+      <c r="K36" s="1">
         <v>42.892095619047616</v>
       </c>
-      <c r="K36" s="1">
+      <c r="L36" s="1">
         <v>-77.285184714285705</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1885,29 +2031,32 @@
       <c r="D37">
         <v>82480</v>
       </c>
-      <c r="E37">
-        <v>372813</v>
-      </c>
-      <c r="F37">
+      <c r="E37" s="5">
+        <v>373551</v>
+      </c>
+      <c r="F37" s="5">
+        <v>374872</v>
+      </c>
+      <c r="G37">
         <v>125925</v>
       </c>
-      <c r="G37" s="2">
+      <c r="H37" s="2">
         <v>2384.5</v>
       </c>
-      <c r="H37" s="2">
+      <c r="I37" s="2">
         <v>259.5</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>2125</v>
       </c>
-      <c r="J37" s="1">
+      <c r="K37" s="1">
         <v>41.388205280701747</v>
       </c>
-      <c r="K37" s="1">
+      <c r="L37" s="1">
         <v>-74.305287368421062</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1920,29 +2069,32 @@
       <c r="D38">
         <v>58535</v>
       </c>
-      <c r="E38">
-        <v>42883</v>
-      </c>
-      <c r="F38">
+      <c r="E38" s="5">
+        <v>42861</v>
+      </c>
+      <c r="F38" s="5">
+        <v>42622</v>
+      </c>
+      <c r="G38">
         <v>16119</v>
       </c>
-      <c r="G38" s="2">
+      <c r="H38" s="2">
         <v>2564.1999999999998</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>190.9</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>2373.3000000000002</v>
       </c>
-      <c r="J38" s="1">
+      <c r="K38" s="1">
         <v>43.307507818181826</v>
       </c>
-      <c r="K38" s="1">
+      <c r="L38" s="1">
         <v>-78.219902636363656</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1955,29 +2107,32 @@
       <c r="D39">
         <v>56364</v>
       </c>
-      <c r="E39">
-        <v>122109</v>
-      </c>
-      <c r="F39">
+      <c r="E39" s="5">
+        <v>122166</v>
+      </c>
+      <c r="F39" s="5">
+        <v>122228</v>
+      </c>
+      <c r="G39">
         <v>46400</v>
       </c>
-      <c r="G39" s="2">
+      <c r="H39" s="2">
         <v>2741.3</v>
       </c>
-      <c r="H39" s="2">
+      <c r="I39" s="2">
         <v>157.6</v>
       </c>
-      <c r="I39" s="2">
+      <c r="J39" s="2">
         <v>2583.6999999999998</v>
       </c>
-      <c r="J39" s="1">
+      <c r="K39" s="1">
         <v>43.425910222222221</v>
       </c>
-      <c r="K39" s="1">
+      <c r="L39" s="1">
         <v>-76.149460037037016</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1990,29 +2145,32 @@
       <c r="D40">
         <v>56797</v>
       </c>
-      <c r="E40">
-        <v>62259</v>
-      </c>
-      <c r="F40">
+      <c r="E40" s="5">
+        <v>62227</v>
+      </c>
+      <c r="F40" s="5">
+        <v>61917</v>
+      </c>
+      <c r="G40">
         <v>24620</v>
       </c>
-      <c r="G40" s="2">
+      <c r="H40" s="2">
         <v>1880</v>
       </c>
-      <c r="H40" s="2">
+      <c r="I40" s="2">
         <v>208.5</v>
       </c>
-      <c r="I40" s="2">
+      <c r="J40" s="2">
         <v>1671.5</v>
       </c>
-      <c r="J40" s="1">
+      <c r="K40" s="1">
         <v>42.626570624999999</v>
       </c>
-      <c r="K40" s="1">
+      <c r="L40" s="1">
         <v>-75.02079268750002</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -2025,29 +2183,32 @@
       <c r="D41">
         <v>101576</v>
       </c>
-      <c r="E41">
-        <v>99710</v>
-      </c>
-      <c r="F41">
+      <c r="E41" s="5">
+        <v>99718</v>
+      </c>
+      <c r="F41" s="5">
+        <v>99933</v>
+      </c>
+      <c r="G41">
         <v>35041</v>
       </c>
-      <c r="G41" s="2">
+      <c r="H41" s="2">
         <v>947.5</v>
       </c>
-      <c r="H41" s="2">
+      <c r="I41" s="2">
         <v>69.099999999999994</v>
       </c>
-      <c r="I41" s="2">
+      <c r="J41" s="2">
         <v>878.4</v>
       </c>
-      <c r="J41" s="1">
+      <c r="K41" s="1">
         <v>41.415569000000005</v>
       </c>
-      <c r="K41" s="1">
+      <c r="L41" s="1">
         <v>-73.761032222222227</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -2060,29 +2221,32 @@
       <c r="D42">
         <v>62459</v>
       </c>
-      <c r="E42">
-        <v>2230722</v>
-      </c>
-      <c r="F42">
+      <c r="E42" s="5">
+        <v>2233895</v>
+      </c>
+      <c r="F42" s="5">
+        <v>2247848</v>
+      </c>
+      <c r="G42">
         <v>780117</v>
       </c>
-      <c r="G42" s="2">
+      <c r="H42" s="2">
         <v>1693.7</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>424.4</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="2">
         <v>1269.3</v>
       </c>
-      <c r="J42" s="1">
+      <c r="K42" s="1">
         <v>40.704546012499996</v>
       </c>
-      <c r="K42" s="1">
+      <c r="L42" s="1">
         <v>-73.830228137499972</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -2095,29 +2259,32 @@
       <c r="D43">
         <v>68390</v>
       </c>
-      <c r="E43">
-        <v>159429</v>
-      </c>
-      <c r="F43">
+      <c r="E43" s="5">
+        <v>159465</v>
+      </c>
+      <c r="F43" s="5">
+        <v>159395</v>
+      </c>
+      <c r="G43">
         <v>64702</v>
       </c>
-      <c r="G43" s="2">
+      <c r="H43" s="2">
         <v>3135.2</v>
       </c>
-      <c r="H43" s="2">
+      <c r="I43" s="2">
         <v>354.3</v>
       </c>
-      <c r="I43" s="2">
+      <c r="J43" s="2">
         <v>2780.9</v>
       </c>
-      <c r="J43" s="1">
+      <c r="K43" s="1">
         <v>42.68491503125</v>
       </c>
-      <c r="K43" s="1">
+      <c r="L43" s="1">
         <v>-73.521919656249992</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -2130,29 +2297,32 @@
       <c r="D44">
         <v>83264</v>
       </c>
-      <c r="E44">
-        <v>468730</v>
-      </c>
-      <c r="F44">
+      <c r="E44" s="5">
+        <v>469393</v>
+      </c>
+      <c r="F44" s="5">
+        <v>470467</v>
+      </c>
+      <c r="G44">
         <v>165516</v>
       </c>
-      <c r="G44" s="2">
+      <c r="H44" s="2">
         <v>1396</v>
       </c>
-      <c r="H44" s="2">
+      <c r="I44" s="2">
         <v>276.60000000000002</v>
       </c>
-      <c r="I44" s="2">
+      <c r="J44" s="2">
         <v>1119.4000000000001</v>
       </c>
-      <c r="J44" s="1">
+      <c r="K44" s="1">
         <v>40.584397714285714</v>
       </c>
-      <c r="K44" s="1">
+      <c r="L44" s="1">
         <v>-74.147875142857146</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -2165,29 +2335,32 @@
       <c r="D45">
         <v>96836</v>
       </c>
-      <c r="E45">
-        <v>311687</v>
-      </c>
-      <c r="F45">
+      <c r="E45" s="5">
+        <v>312520</v>
+      </c>
+      <c r="F45" s="5">
+        <v>315158</v>
+      </c>
+      <c r="G45">
         <v>99242</v>
       </c>
-      <c r="G45" s="2">
+      <c r="H45" s="2">
         <v>1596.8</v>
       </c>
-      <c r="H45" s="2">
+      <c r="I45" s="2">
         <v>154.30000000000001</v>
       </c>
-      <c r="I45" s="2">
+      <c r="J45" s="2">
         <v>1442.5</v>
       </c>
-      <c r="J45" s="1">
+      <c r="K45" s="1">
         <v>41.131479642857137</v>
       </c>
-      <c r="K45" s="1">
+      <c r="L45" s="1">
         <v>-74.012710749999997</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -2200,29 +2373,32 @@
       <c r="D46">
         <v>81251</v>
       </c>
-      <c r="E46">
-        <v>219607</v>
-      </c>
-      <c r="F46">
+      <c r="E46" s="5">
+        <v>111917</v>
+      </c>
+      <c r="F46" s="5">
+        <v>111690</v>
+      </c>
+      <c r="G46">
         <v>88296</v>
       </c>
-      <c r="G46" s="2">
+      <c r="H46" s="2">
         <v>2219.4</v>
       </c>
-      <c r="H46" s="2">
+      <c r="I46" s="2">
         <v>127.5</v>
       </c>
-      <c r="I46" s="2">
+      <c r="J46" s="2">
         <v>2091.9</v>
       </c>
-      <c r="J46" s="1">
+      <c r="K46" s="1">
         <v>42.959001999999998</v>
       </c>
-      <c r="K46" s="1">
+      <c r="L46" s="1">
         <v>-73.865754500000008</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -2235,29 +2411,32 @@
       <c r="D47">
         <v>70712</v>
       </c>
-      <c r="E47">
-        <v>154727</v>
-      </c>
-      <c r="F47">
+      <c r="E47" s="5">
+        <v>219988</v>
+      </c>
+      <c r="F47" s="5">
+        <v>220882</v>
+      </c>
+      <c r="G47">
         <v>62886</v>
       </c>
-      <c r="G47" s="2">
+      <c r="H47" s="2">
         <v>1474.1</v>
       </c>
-      <c r="H47" s="2">
+      <c r="I47" s="2">
         <v>68.8</v>
       </c>
-      <c r="I47" s="2">
+      <c r="J47" s="2">
         <v>1405.3</v>
       </c>
-      <c r="J47" s="1">
+      <c r="K47" s="1">
         <v>43.066152952380946</v>
       </c>
-      <c r="K47" s="1">
+      <c r="L47" s="1">
         <v>-73.827062904761917</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -2270,29 +2449,32 @@
       <c r="D48">
         <v>61828</v>
       </c>
-      <c r="E48">
-        <v>32749</v>
-      </c>
-      <c r="F48">
+      <c r="E48" s="5">
+        <v>154932</v>
+      </c>
+      <c r="F48" s="5">
+        <v>155058</v>
+      </c>
+      <c r="G48">
         <v>13166</v>
       </c>
-      <c r="G48" s="2">
+      <c r="H48" s="2">
         <v>3984.5</v>
       </c>
-      <c r="H48" s="2">
+      <c r="I48" s="2">
         <v>494.6</v>
       </c>
-      <c r="I48" s="2">
+      <c r="J48" s="2">
         <v>3489.9</v>
       </c>
-      <c r="J48" s="1">
+      <c r="K48" s="1">
         <v>42.816311411764708</v>
       </c>
-      <c r="K48" s="1">
+      <c r="L48" s="1">
         <v>-74.016709470588239</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -2305,29 +2487,32 @@
       <c r="D49">
         <v>54322</v>
       </c>
-      <c r="E49">
-        <v>18343</v>
-      </c>
-      <c r="F49">
+      <c r="E49" s="5">
+        <v>32692</v>
+      </c>
+      <c r="F49" s="5">
+        <v>32578</v>
+      </c>
+      <c r="G49">
         <v>7530</v>
       </c>
-      <c r="G49" s="2">
+      <c r="H49" s="2">
         <v>1498.3</v>
       </c>
-      <c r="H49" s="2">
+      <c r="I49" s="2">
         <v>54.5</v>
       </c>
-      <c r="I49" s="2">
+      <c r="J49" s="2">
         <v>1443.7</v>
       </c>
-      <c r="J49" s="1">
+      <c r="K49" s="1">
         <v>42.608253166666664</v>
       </c>
-      <c r="K49" s="1">
+      <c r="L49" s="1">
         <v>-74.460739166666656</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -2340,29 +2525,32 @@
       <c r="D50">
         <v>53857</v>
       </c>
-      <c r="E50">
-        <v>35251</v>
-      </c>
-      <c r="F50">
+      <c r="E50" s="5">
+        <v>18338</v>
+      </c>
+      <c r="F50" s="5">
+        <v>18361</v>
+      </c>
+      <c r="G50">
         <v>13393</v>
       </c>
-      <c r="G50" s="2">
+      <c r="H50" s="2">
         <v>1067.5</v>
       </c>
-      <c r="H50" s="2">
+      <c r="I50" s="2">
         <v>54.2</v>
       </c>
-      <c r="I50" s="2">
+      <c r="J50" s="2">
         <v>1013.3</v>
       </c>
-      <c r="J50" s="1">
+      <c r="K50" s="1">
         <v>42.399321249999993</v>
       </c>
-      <c r="K50" s="1">
+      <c r="L50" s="1">
         <v>-76.860707083333338</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -2375,29 +2563,32 @@
       <c r="D51">
         <v>50384</v>
       </c>
-      <c r="E51">
-        <v>111944</v>
-      </c>
-      <c r="F51">
+      <c r="E51" s="5">
+        <v>35206</v>
+      </c>
+      <c r="F51" s="5">
+        <v>35198</v>
+      </c>
+      <c r="G51">
         <v>41605</v>
       </c>
-      <c r="G51" s="2">
+      <c r="H51" s="2">
         <v>1944.3</v>
       </c>
-      <c r="H51" s="2">
+      <c r="I51" s="2">
         <v>154.1</v>
       </c>
-      <c r="I51" s="2">
+      <c r="J51" s="2">
         <v>1790.2</v>
       </c>
-      <c r="J51" s="1">
+      <c r="K51" s="1">
         <v>42.742238249999993</v>
       </c>
-      <c r="K51" s="1">
+      <c r="L51" s="1">
         <v>-76.815980749999994</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -2410,29 +2601,32 @@
       <c r="D52">
         <v>52867</v>
       </c>
-      <c r="E52">
-        <v>98990</v>
-      </c>
-      <c r="F52">
+      <c r="E52" s="5">
+        <v>98938</v>
+      </c>
+      <c r="F52" s="5">
+        <v>99033</v>
+      </c>
+      <c r="G52">
         <v>40344</v>
       </c>
-      <c r="G52" s="2">
+      <c r="H52" s="2">
         <v>1928.6</v>
       </c>
-      <c r="H52" s="2">
+      <c r="I52" s="2">
         <v>172.2</v>
       </c>
-      <c r="I52" s="2">
+      <c r="J52" s="2">
         <v>1756.4</v>
       </c>
-      <c r="J52" s="1">
+      <c r="K52" s="1">
         <v>42.286168517241379</v>
       </c>
-      <c r="K52" s="1">
+      <c r="L52" s="1">
         <v>-77.382201689655176</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -2445,29 +2639,32 @@
       <c r="D53">
         <v>96220</v>
       </c>
-      <c r="E53">
-        <v>1493350</v>
-      </c>
-      <c r="F53">
+      <c r="E53" s="5">
+        <v>1494388</v>
+      </c>
+      <c r="F53" s="5">
+        <v>1498816</v>
+      </c>
+      <c r="G53">
         <v>499922</v>
       </c>
-      <c r="G53" s="2">
+      <c r="H53" s="2">
         <v>2158.6</v>
       </c>
-      <c r="H53" s="2">
+      <c r="I53" s="2">
         <v>157.30000000000001</v>
       </c>
-      <c r="I53" s="2">
+      <c r="J53" s="2">
         <v>2001.3</v>
       </c>
-      <c r="J53" s="1">
+      <c r="K53" s="1">
         <v>40.870803974358914</v>
       </c>
-      <c r="K53" s="1">
+      <c r="L53" s="1">
         <v>-72.860682837606745</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -2480,29 +2677,32 @@
       <c r="D54">
         <v>57388</v>
       </c>
-      <c r="E54">
-        <v>77547</v>
-      </c>
-      <c r="F54">
+      <c r="E54" s="5">
+        <v>77470</v>
+      </c>
+      <c r="F54" s="5">
+        <v>76900</v>
+      </c>
+      <c r="G54">
         <v>30139</v>
       </c>
-      <c r="G54" s="2">
+      <c r="H54" s="2">
         <v>2270.5</v>
       </c>
-      <c r="H54" s="2">
+      <c r="I54" s="2">
         <v>290.10000000000002</v>
       </c>
-      <c r="I54" s="2">
+      <c r="J54" s="2">
         <v>1980.4</v>
       </c>
-      <c r="J54" s="1">
+      <c r="K54" s="1">
         <v>41.711774821428556</v>
       </c>
-      <c r="K54" s="1">
+      <c r="L54" s="1">
         <v>-74.784253142857125</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -2515,29 +2715,32 @@
       <c r="D55">
         <v>59907</v>
       </c>
-      <c r="E55">
-        <v>51125</v>
-      </c>
-      <c r="F55">
+      <c r="E55" s="5">
+        <v>51095</v>
+      </c>
+      <c r="F55" s="5">
+        <v>51043</v>
+      </c>
+      <c r="G55">
         <v>20350</v>
       </c>
-      <c r="G55" s="2">
+      <c r="H55" s="2">
         <v>1135</v>
       </c>
-      <c r="H55" s="2">
+      <c r="I55" s="2">
         <v>73</v>
       </c>
-      <c r="I55" s="2">
+      <c r="J55" s="2">
         <v>1062</v>
       </c>
-      <c r="J55" s="1">
+      <c r="K55" s="1">
         <v>42.155233857142854</v>
       </c>
-      <c r="K55" s="1">
+      <c r="L55" s="1">
         <v>-76.338944928571436</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -2550,29 +2753,32 @@
       <c r="D56">
         <v>72231</v>
       </c>
-      <c r="E56">
-        <v>101564</v>
-      </c>
-      <c r="F56">
+      <c r="E56" s="5">
+        <v>101654</v>
+      </c>
+      <c r="F56" s="5">
+        <v>101723</v>
+      </c>
+      <c r="G56">
         <v>38967</v>
       </c>
-      <c r="G56" s="2">
+      <c r="H56" s="2">
         <v>2475.3000000000002</v>
       </c>
-      <c r="H56" s="2">
+      <c r="I56" s="2">
         <v>118.6</v>
       </c>
-      <c r="I56" s="2">
+      <c r="J56" s="2">
         <v>2356.6999999999998</v>
       </c>
-      <c r="J56" s="1">
+      <c r="K56" s="1">
         <v>42.469065799999996</v>
       </c>
-      <c r="K56" s="1">
+      <c r="L56" s="1">
         <v>-76.452987933333347</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -2585,29 +2791,32 @@
       <c r="D57">
         <v>70513</v>
       </c>
-      <c r="E57">
-        <v>182493</v>
-      </c>
-      <c r="F57">
+      <c r="E57" s="5">
+        <v>182473</v>
+      </c>
+      <c r="F57" s="5">
+        <v>182448</v>
+      </c>
+      <c r="G57">
         <v>71049</v>
       </c>
-      <c r="G57" s="2">
+      <c r="H57" s="2">
         <v>2135.6</v>
       </c>
-      <c r="H57" s="2">
+      <c r="I57" s="2">
         <v>227</v>
       </c>
-      <c r="I57" s="2">
+      <c r="J57" s="2">
         <v>1908.6</v>
       </c>
-      <c r="J57" s="1">
+      <c r="K57" s="1">
         <v>41.880661775862059</v>
       </c>
-      <c r="K57" s="1">
+      <c r="L57" s="1">
         <v>-74.176534620689665</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -2620,29 +2829,32 @@
       <c r="D58">
         <v>64195</v>
       </c>
-      <c r="E58">
-        <v>65707</v>
-      </c>
-      <c r="F58">
+      <c r="E58" s="5">
+        <v>65723</v>
+      </c>
+      <c r="F58" s="5">
+        <v>65831</v>
+      </c>
+      <c r="G58">
         <v>27990</v>
       </c>
-      <c r="G58" s="2">
+      <c r="H58" s="2">
         <v>1961.9</v>
       </c>
-      <c r="H58" s="2">
+      <c r="I58" s="2">
         <v>146.5</v>
       </c>
-      <c r="I58" s="2">
+      <c r="J58" s="2">
         <v>1815.4</v>
       </c>
-      <c r="J58" s="1">
+      <c r="K58" s="1">
         <v>43.577636043478257</v>
       </c>
-      <c r="K58" s="1">
+      <c r="L58" s="1">
         <v>-73.805926391304354</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -2655,29 +2867,32 @@
       <c r="D59">
         <v>57360</v>
       </c>
-      <c r="E59">
-        <v>63216</v>
-      </c>
-      <c r="F59">
+      <c r="E59" s="5">
+        <v>63322</v>
+      </c>
+      <c r="F59" s="5">
+        <v>63165</v>
+      </c>
+      <c r="G59">
         <v>24142</v>
       </c>
-      <c r="G59" s="3">
+      <c r="H59" s="3">
         <v>1412.6</v>
       </c>
-      <c r="H59" s="3">
+      <c r="I59" s="3">
         <v>149.5</v>
       </c>
-      <c r="I59" s="3">
+      <c r="J59" s="3">
         <v>1263.0999999999999</v>
       </c>
-      <c r="J59" s="4">
+      <c r="K59" s="4">
         <v>43.343649666666664</v>
       </c>
-      <c r="K59" s="4">
+      <c r="L59" s="4">
         <v>-73.409863380952373</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -2690,29 +2905,32 @@
       <c r="D60">
         <v>60324</v>
       </c>
-      <c r="E60">
-        <v>93772</v>
-      </c>
-      <c r="F60">
+      <c r="E60" s="5">
+        <v>93783</v>
+      </c>
+      <c r="F60" s="5">
+        <v>93436</v>
+      </c>
+      <c r="G60">
         <v>36585</v>
       </c>
-      <c r="G60" s="2">
+      <c r="H60" s="2">
         <v>2171.6</v>
       </c>
-      <c r="H60" s="2">
+      <c r="I60" s="2">
         <v>186.6</v>
       </c>
-      <c r="I60" s="2">
+      <c r="J60" s="2">
         <v>1985</v>
       </c>
-      <c r="J60" s="1">
+      <c r="K60" s="1">
         <v>43.189853363636374</v>
       </c>
-      <c r="K60" s="1">
+      <c r="L60" s="1">
         <v>-77.031195227272732</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -2725,29 +2943,32 @@
       <c r="D61">
         <v>100863</v>
       </c>
-      <c r="E61">
-        <v>949113</v>
-      </c>
-      <c r="F61">
+      <c r="E61" s="5">
+        <v>950283</v>
+      </c>
+      <c r="F61" s="5">
+        <v>955899</v>
+      </c>
+      <c r="G61">
         <v>347232</v>
       </c>
-      <c r="G61" s="2">
+      <c r="H61" s="2">
         <v>1615.5</v>
       </c>
-      <c r="H61" s="2">
+      <c r="I61" s="2">
         <v>258.8</v>
       </c>
-      <c r="I61" s="2">
+      <c r="J61" s="2">
         <v>1356.7</v>
       </c>
-      <c r="J61" s="1">
+      <c r="K61" s="1">
         <v>41.11656854347828</v>
       </c>
-      <c r="K61" s="1">
+      <c r="L61" s="1">
         <v>-73.775226076086952</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -2760,29 +2981,32 @@
       <c r="D62">
         <v>58009</v>
       </c>
-      <c r="E62">
-        <v>42155</v>
-      </c>
-      <c r="F62">
+      <c r="E62" s="5">
+        <v>42138</v>
+      </c>
+      <c r="F62" s="5">
+        <v>41944</v>
+      </c>
+      <c r="G62">
         <v>15501</v>
       </c>
-      <c r="G62" s="2">
+      <c r="H62" s="2">
         <v>1168.3</v>
       </c>
-      <c r="H62" s="2">
+      <c r="I62" s="2">
         <v>81</v>
       </c>
-      <c r="I62" s="2">
+      <c r="J62" s="2">
         <v>1087.3</v>
       </c>
-      <c r="J62" s="1">
+      <c r="K62" s="1">
         <v>42.681614947368423</v>
       </c>
-      <c r="K62" s="1">
+      <c r="L62" s="1">
         <v>-78.229685631578946</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -2795,25 +3019,28 @@
       <c r="D63">
         <v>56538</v>
       </c>
-      <c r="E63">
-        <v>25348</v>
-      </c>
-      <c r="F63">
+      <c r="E63" s="6">
+        <v>25367</v>
+      </c>
+      <c r="F63" s="6">
+        <v>25454</v>
+      </c>
+      <c r="G63">
         <v>9517</v>
       </c>
-      <c r="G63" s="2">
+      <c r="H63" s="2">
         <v>1960.1</v>
       </c>
-      <c r="H63" s="2">
+      <c r="I63" s="2">
         <v>74.400000000000006</v>
       </c>
-      <c r="I63" s="2">
+      <c r="J63" s="2">
         <v>1885.7</v>
       </c>
-      <c r="J63" s="1">
+      <c r="K63" s="1">
         <v>42.623117909090908</v>
       </c>
-      <c r="K63" s="1">
+      <c r="L63" s="1">
         <v>-77.069860272727283</v>
       </c>
     </row>
@@ -2883,6 +3110,11 @@
     <hyperlink ref="A63" r:id="rId62" tooltip="Yates County, New York"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2892,9 +3124,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2904,8 +3141,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>